<commit_message>
Mejorar la visualización de errores en la página de calibraciones: agregar tablas de error absoluto y relativo, y mejorar la presentación de gráficos.
</commit_message>
<xml_diff>
--- a/data/mediciones_x3.xlsx
+++ b/data/mediciones_x3.xlsx
@@ -113,7 +113,7 @@
     <t>DUT3_R</t>
   </si>
   <si>
-    <t>PAT3_270</t>
+    <t>PAT3_0</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,6 +1469,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="24"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="25" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L25" s="23"/>

</xml_diff>